<commit_message>
Template update for 700 sessions
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
+++ b/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
@@ -604,8 +604,8 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
template update and fixed encoding for store variable
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
+++ b/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">SOVI SSD GELADO KO</t>
   </si>
   <si>
-    <t xml:space="preserve">Balcão Refrigerado – PDV, Geladeira – CONC, Geladeira – KO, GELADEIRA - PDV</t>
+    <t xml:space="preserve">Balcão Refrigerado – PDV, Geladeira – CONC, Geladeira – KO, GELADEIRA – PDV</t>
   </si>
   <si>
     <t xml:space="preserve">LOJA DE CONVENIÊNCIA,RESTAURANTE AB,RESTAURANTE C,BAR BOTECO AB,BAR BOTECO C,BAR LANCHONETE AB,BAR LANCHONETE C,MERCEARIA,PADARIA C,AS 1-4,AS 5+</t>
@@ -405,7 +405,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +416,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2F5597"/>
         <bgColor rgb="FF555555"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -472,12 +478,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,18 +507,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,19 +515,31 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -604,15 +622,15 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.5546558704453"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="170.105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.3036437246964"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.7408906882591"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -630,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -645,48 +663,48 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" s="9" customFormat="true" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -700,7 +718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -714,7 +732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="4" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -729,34 +747,34 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" s="6" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" s="9" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -770,7 +788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -784,63 +802,63 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+    <row r="13" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -854,21 +872,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+    <row r="18" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -882,14 +900,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+    <row r="20" s="4" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -897,20 +915,20 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -925,44 +943,44 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="D24" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -984,22 +1002,22 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.3765182186235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.0202429149798"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1036,10 +1054,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1056,10 +1074,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -1076,10 +1094,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -1096,10 +1114,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="27.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -1122,10 +1140,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -1148,10 +1166,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1168,10 +1186,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -1188,10 +1206,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -1208,10 +1226,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1228,10 +1246,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -1248,10 +1266,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -1268,10 +1286,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -1288,10 +1306,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -1314,10 +1332,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -1329,7 +1347,7 @@
       <c r="E15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="11" t="s">
         <v>84</v>
       </c>
       <c r="I15" s="0" t="s">
@@ -1340,10 +1358,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C16" s="0" t="s">
@@ -1355,7 +1373,7 @@
       <c r="E16" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="11" t="s">
         <v>84</v>
       </c>
       <c r="I16" s="0" t="s">
@@ -1366,10 +1384,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C17" s="0" t="s">
@@ -1378,40 +1396,40 @@
       <c r="D17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="12" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" s="10" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+    <row r="18" s="12" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10" t="s">
+      <c r="C18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -1433,39 +1451,39 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" s="10" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+    <row r="20" s="12" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="10" t="s">
+      <c r="C20" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="10" t="s">
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
@@ -1488,10 +1506,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C22" s="0" t="s">
@@ -1514,10 +1532,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -1532,7 +1550,7 @@
       <c r="F23" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="12" t="s">
         <v>69</v>
       </c>
       <c r="J23" s="0" t="s">
@@ -1540,10 +1558,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C24" s="0" t="s">
@@ -1572,10 +1590,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="0" t="s">

</xml_diff>

<commit_message>
Geladeira - pdv fixed in template
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
+++ b/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">SOVI SSD GELADO KO</t>
   </si>
   <si>
-    <t xml:space="preserve">Balcão Refrigerado – PDV, Geladeira – CONC, Geladeira – KO, GELADEIRA – PDV</t>
+    <t xml:space="preserve">Balcão Refrigerado – PDV, Geladeira – CONC, Geladeira – PDV, Geladeira – KO</t>
   </si>
   <si>
     <t xml:space="preserve">LOJA DE CONVENIÊNCIA,RESTAURANTE AB,RESTAURANTE C,BAR BOTECO AB,BAR BOTECO C,BAR LANCHONETE AB,BAR LANCHONETE C,MERCEARIA,PADARIA C,AS 1-4,AS 5+</t>
@@ -623,7 +623,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -690,11 +690,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" s="9" customFormat="true" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -764,7 +764,7 @@
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -806,7 +806,7 @@
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -848,7 +848,7 @@
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">

</xml_diff>

<commit_message>
Template update PROS 7206 and PROS 7131
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
+++ b/Projects/SOLARBR/Data/KPI Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="102">
   <si>
     <t xml:space="preserve">KPI NAME</t>
   </si>
@@ -103,13 +103,13 @@
     <t xml:space="preserve">SOVI SSD SABORES KO</t>
   </si>
   <si>
-    <t xml:space="preserve">MERCEARIA,AS 1-4,AS 5+,ATACADO</t>
+    <t xml:space="preserve">MERCEARIA,AS 1-4,AS 5+,ATACADO,PADARIA AB,PADARIA C</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI ÁGUA</t>
   </si>
   <si>
-    <t xml:space="preserve">DROGARIA,MERCEARIA,PADARIA AB,PADARIA C,AS 1-4,AS 5+,ATACADO</t>
+    <t xml:space="preserve">DROGARIA,MERCEARIA,PADARIA AB,PADARIA C,AS 1-4,AS 5+,ATACADO,LOJA DE CONVENIÊNCIA</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI STILL KO</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">SOVI ENERGETICO</t>
   </si>
   <si>
-    <t xml:space="preserve">DROGARIA,LOJA DE CONVENIÊNCIA,AS 5+,ATACADO</t>
+    <t xml:space="preserve">LOJA DE CONVENIÊNCIA,AS 5+,ATACADO</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI CERVEJA</t>
@@ -298,58 +298,61 @@
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
+    <t xml:space="preserve">Coca-Cola,Coca Cola Stevia,Coca-Cola Zero,Coca-Cola Cafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of the folowing products (REFPET CC, LS CC, LS FANTA, LS JESUS, LS KUAT, REFPET CC ZERO, REFPET FANTA LARANJA) and size greater than 600ml  / Quantity total of products of the category SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DePara Categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retornavel Familiar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of products of the categories STILL and manufacturer Coca Cola / Quantity total of products of the categories STILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of products of the sub brand Guarana and manufacturer Coca Cola / Quantity total of products of the sub brand Laranja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laranja,Guaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of the folowing Brands (AQUARIUS, COCA COLA, FANTA, JESUS, KUAT, SCHWEPPES, SPRITE) and size lower or equal than 600ml  / Quantity total of products of the category SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350.0,500.0,200.0,300.0,330.0,260.0,473.0,600.0,355.0,250.0,269.0,310.0,450.0,290.0,1.5,1.0,220.0,2.0,3.3,237.0,2.5,510.0,497.0,6.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of products of the brand ADES, subcategory SOJA and manufacturer Coca Cola / Quantity total of products of the subcategory SOJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of products of a specific list of products in the category SSD and manufacturer Coca Cola / Quantity total of products of the category SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero, Coca Cola Stevia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coca-Cola,Coca Cola Stevia,Coca-Cola Zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity of the folowing products (REFPET CC, LS CC, LS FANTA, LS JESUS, LS KUAT, REFPET CC ZERO, REFPET FANTA LARANJA) and size greater than 600ml  / Quantity total of products of the category SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DePara Categoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retornavel Familiar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity of products of the categories STILL and manufacturer Coca Cola / Quantity total of products of the categories STILL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity of products of the sub brand Guarana and manufacturer Coca Cola / Quantity total of products of the sub brand Laranja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub_brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laranja,Guaran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity of the folowing Brands (AQUARIUS, COCA COLA, FANTA, JESUS, KUAT, SCHWEPPES, SPRITE) and size lower or equal than 600ml  / Quantity total of products of the category SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">350.0,500.0,200.0,300.0,330.0,260.0,473.0,600.0,355.0,250.0,269.0,310.0,450.0,290.0,1.5,1.0,220.0,2.0,3.3,237.0,2.5,510.0,497.0,6.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity of products of the brand ADES, subcategory SOJA and manufacturer Coca Cola / Quantity total of products of the subcategory SOJA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity of products of a specific list of products in the category SSD and manufacturer Coca Cola / Quantity total of products of the category SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero, Coca Cola Stevia</t>
   </si>
   <si>
     <t xml:space="preserve">Ponto extra - Setor de bebidas</t>
@@ -481,7 +484,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -524,10 +527,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -633,15 +632,15 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.4858299595142"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="86.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1013,22 +1012,22 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.4858299595142"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1146,7 +1145,7 @@
       <c r="I5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1358,7 +1357,7 @@
       <c r="E15" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>85</v>
       </c>
       <c r="I15" s="0" t="s">
@@ -1384,7 +1383,7 @@
       <c r="E16" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>85</v>
       </c>
       <c r="I16" s="0" t="s">
@@ -1407,32 +1406,32 @@
       <c r="D17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="13" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
+    <row r="18" s="13" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="14" t="s">
+      <c r="C18" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="13" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1462,31 +1461,31 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" s="14" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+    <row r="20" s="13" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="14" t="s">
+      <c r="C20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="14" t="s">
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1523,25 +1522,25 @@
       <c r="B22" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="C22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="J22" s="12" t="s">
-        <v>82</v>
+      <c r="J22" s="11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,7 +1562,7 @@
       <c r="F23" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>69</v>
       </c>
       <c r="J23" s="0" t="s">
@@ -1619,7 +1618,7 @@
         <v>97</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>66</v>

</xml_diff>